<commit_message>
Ajustes final para Mirlaine
</commit_message>
<xml_diff>
--- a/atendente/sorteios_exportados.xlsx
+++ b/atendente/sorteios_exportados.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>cpf</t>
   </si>
@@ -22,16 +22,22 @@
     <t>premio</t>
   </si>
   <si>
-    <t>data</t>
+    <t>data_sorteio</t>
+  </si>
+  <si>
+    <t>atendente_cadastro</t>
   </si>
   <si>
     <t>13692306644</t>
   </si>
   <si>
-    <t>Check-up Básico</t>
-  </si>
-  <si>
-    <t>2025-08-06T17:03:00.036375</t>
+    <t>Consulta Odontológica Bonificada</t>
+  </si>
+  <si>
+    <t>08/08/2025 16:36:11</t>
+  </si>
+  <si>
+    <t>Lucas Mendes</t>
   </si>
 </sst>
 </file>
@@ -389,13 +395,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -405,16 +411,22 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>